<commit_message>
Red Line Connections Set Up
</commit_message>
<xml_diff>
--- a/CTC_App/Iteration3/Track_Layout_Red.xlsx
+++ b/CTC_App/Iteration3/Track_Layout_Red.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yasse\Desktop\ECE1140\Team_X_ECE_1140\CTC_App\Iteration3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D401C14-19C5-464D-A7C3-0367EEA53E6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AB8D9E-0A6F-425E-ABC9-1DA0C0B8066E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8424" yWindow="0" windowWidth="9348" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20472" yWindow="-36" windowWidth="4572" windowHeight="11748" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Red Line" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="44">
   <si>
     <t>Line</t>
   </si>
@@ -89,15 +89,9 @@
     <t>G</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>J</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -153,13 +147,34 @@
   </si>
   <si>
     <t>SOUTH HILLS JUNCTION L</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -188,6 +203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -556,9 +577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMF152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="54" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I44" sqref="I44"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="B18:G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -606,7 +627,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -635,7 +656,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>10</v>
@@ -836,7 +857,7 @@
         <v>-1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I9" s="2">
         <v>-1</v>
@@ -1106,7 +1127,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I18" s="2">
         <v>-1</v>
@@ -1256,7 +1277,7 @@
         <v>-1</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="I23" s="2">
         <v>-1</v>
@@ -1328,7 +1349,7 @@
         <v>Red</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C26" s="9">
         <v>24</v>
@@ -1358,7 +1379,7 @@
         <v>Red</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C27" s="10">
         <v>25</v>
@@ -1376,7 +1397,7 @@
         <v>-1</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I27" s="2">
         <v>-1</v>
@@ -1388,7 +1409,7 @@
         <v>Red</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C28" s="9">
         <v>26</v>
@@ -1418,7 +1439,7 @@
         <v>Red</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C29" s="10">
         <v>27</v>
@@ -1448,7 +1469,7 @@
         <v>Red</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C30" s="9">
         <v>28</v>
@@ -1478,7 +1499,7 @@
         <v>Red</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C31" s="9">
         <v>29</v>
@@ -1508,7 +1529,7 @@
         <v>Red</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C32" s="10">
         <v>30</v>
@@ -1538,7 +1559,7 @@
         <v>Red</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C33" s="9">
         <v>31</v>
@@ -1568,7 +1589,7 @@
         <v>Red</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="C34" s="10">
         <v>32</v>
@@ -1598,7 +1619,7 @@
         <v>Red</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C35" s="9">
         <v>33</v>
@@ -1628,7 +1649,7 @@
         <v>Red</v>
       </c>
       <c r="B36" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C36" s="9">
         <v>34</v>
@@ -1658,7 +1679,7 @@
         <v>Red</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C37" s="10">
         <v>35</v>
@@ -1676,7 +1697,7 @@
         <v>-1</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="I37" s="2">
         <v>-1</v>
@@ -1688,7 +1709,7 @@
         <v>Red</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C38" s="9">
         <v>36</v>
@@ -1718,7 +1739,7 @@
         <v>Red</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C39" s="9">
         <v>37</v>
@@ -1748,7 +1769,7 @@
         <v>Red</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C40" s="10">
         <v>38</v>
@@ -1778,7 +1799,7 @@
         <v>Red</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C41" s="9">
         <v>39</v>
@@ -1808,7 +1829,7 @@
         <v>Red</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C42" s="9">
         <v>40</v>
@@ -1838,7 +1859,7 @@
         <v>Red</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C43" s="10">
         <v>41</v>
@@ -1868,7 +1889,7 @@
         <v>Red</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C44" s="9">
         <v>42</v>
@@ -1898,7 +1919,7 @@
         <v>Red</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C45" s="9">
         <v>43</v>
@@ -1928,7 +1949,7 @@
         <v>Red</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C46" s="10">
         <v>44</v>
@@ -1958,7 +1979,7 @@
         <v>Red</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="C47" s="9">
         <v>45</v>
@@ -1976,7 +1997,7 @@
         <v>-1</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I47" s="2">
         <v>-1</v>
@@ -1988,7 +2009,7 @@
         <v>Red</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C48" s="9">
         <v>46</v>
@@ -2018,7 +2039,7 @@
         <v>Red</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C49" s="10">
         <v>47</v>
@@ -2048,7 +2069,7 @@
         <v>Red</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C50" s="9">
         <v>48</v>
@@ -2066,7 +2087,7 @@
         <v>-1</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I50" s="2">
         <v>-1</v>
@@ -2078,7 +2099,7 @@
         <v>Red</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C51" s="9">
         <v>49</v>
@@ -2108,7 +2129,7 @@
         <v>Red</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C52" s="10">
         <v>50</v>
@@ -2138,7 +2159,7 @@
         <v>Red</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C53" s="9">
         <v>51</v>
@@ -2168,7 +2189,7 @@
         <v>Red</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="C54" s="9">
         <v>52</v>
@@ -2198,7 +2219,7 @@
         <v>Red</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C55" s="10">
         <v>53</v>
@@ -2228,7 +2249,7 @@
         <v>Red</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="C56" s="9">
         <v>54</v>
@@ -2258,7 +2279,7 @@
         <v>Red</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C57" s="9">
         <v>55</v>
@@ -2288,7 +2309,7 @@
         <v>Red</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C58" s="10">
         <v>56</v>
@@ -2318,7 +2339,7 @@
         <v>Red</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C59" s="9">
         <v>57</v>
@@ -2348,7 +2369,7 @@
         <v>Red</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C60" s="9">
         <v>58</v>
@@ -2378,7 +2399,7 @@
         <v>Red</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C61" s="10">
         <v>59</v>
@@ -2408,7 +2429,7 @@
         <v>Red</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C62" s="9">
         <v>60</v>
@@ -2426,7 +2447,7 @@
         <v>-1</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I62" s="2">
         <v>-1</v>
@@ -2438,7 +2459,7 @@
         <v>Red</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C63" s="9">
         <v>61</v>
@@ -2468,7 +2489,7 @@
         <v>Red</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C64" s="10">
         <v>62</v>
@@ -2498,7 +2519,7 @@
         <v>Red</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C65" s="9">
         <v>63</v>
@@ -2528,7 +2549,7 @@
         <v>Red</v>
       </c>
       <c r="B66" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C66" s="9">
         <v>64</v>
@@ -2558,7 +2579,7 @@
         <v>Red</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C67" s="10">
         <v>65</v>
@@ -2588,7 +2609,7 @@
         <v>Red</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C68" s="9">
         <v>66</v>
@@ -2618,7 +2639,7 @@
         <v>Red</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C69" s="9">
         <v>67</v>
@@ -2648,7 +2669,7 @@
         <v>Red</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C70" s="10">
         <v>68</v>
@@ -2678,7 +2699,7 @@
         <v>Red</v>
       </c>
       <c r="B71" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C71" s="9">
         <v>69</v>
@@ -2708,7 +2729,7 @@
         <v>Red</v>
       </c>
       <c r="B72" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C72" s="9">
         <v>70</v>
@@ -2738,7 +2759,7 @@
         <v>Red</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C73" s="10">
         <v>71</v>
@@ -2768,7 +2789,7 @@
         <v>Red</v>
       </c>
       <c r="B74" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C74" s="9">
         <v>72</v>
@@ -2798,7 +2819,7 @@
         <v>Red</v>
       </c>
       <c r="B75" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C75" s="9">
         <v>73</v>
@@ -2828,7 +2849,7 @@
         <v>Red</v>
       </c>
       <c r="B76" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C76" s="10">
         <v>74</v>
@@ -2858,7 +2879,7 @@
         <v>Red</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C77" s="9">
         <v>75</v>
@@ -2888,7 +2909,7 @@
         <v>Red</v>
       </c>
       <c r="B78" s="9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C78" s="9">
         <v>76</v>
@@ -2999,6 +3020,7 @@
       <c r="C152" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>